<commit_message>
changes in flight validation
</commit_message>
<xml_diff>
--- a/src/test/java/resource/viadata.xlsx
+++ b/src/test/java/resource/viadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Garuda</t>
   </si>
   <si>
-    <t>SuplierName</t>
-  </si>
-  <si>
     <t>AirAsia</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
   </si>
   <si>
     <t>28/Apr/2024</t>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,13 +472,12 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="39.5703125"/>
     <col min="6" max="6" customWidth="true" width="14.0"/>
     <col min="7" max="7" customWidth="true" width="14.42578125"/>
-    <col min="8" max="8" customWidth="true" width="13.42578125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.06640625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.06640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -496,18 +495,15 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -525,18 +521,15 @@
         <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -545,10 +538,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>23</v>
@@ -556,16 +549,13 @@
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -574,21 +564,18 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes in excel data
</commit_message>
<xml_diff>
--- a/src/test/java/resource/viadata.xlsx
+++ b/src/test/java/resource/viadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -92,19 +92,25 @@
     <t>Ramesh</t>
   </si>
   <si>
-    <t>28/Apr/2024</t>
-  </si>
-  <si>
-    <t>29/Apr/2024</t>
-  </si>
-  <si>
-    <t>30/Apr/2024</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>28/Mei/2024</t>
+  </si>
+  <si>
+    <t>29/Mei/2024</t>
+  </si>
+  <si>
+    <t>30/Mei/2024</t>
+  </si>
+  <si>
+    <t>23/Mei/2024</t>
   </si>
 </sst>
 </file>
@@ -112,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +134,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +186,26 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -170,13 +236,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +575,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -518,17 +591,17 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>25</v>
+      <c r="H2" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -543,18 +616,18 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>23</v>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>25</v>
+      <c r="H3" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -569,14 +642,40 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>24</v>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>26</v>
+      <c r="H4" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change for date selection
</commit_message>
<xml_diff>
--- a/src/test/java/resource/viadata.xlsx
+++ b/src/test/java/resource/viadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>28/Mei/2024</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
   </si>
   <si>
     <t>30/Mei/2024</t>
-  </si>
-  <si>
-    <t>23/Mei/2024</t>
   </si>
 </sst>
 </file>
@@ -118,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,9 +144,19 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -236,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -245,11 +249,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,12 +597,12 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -617,12 +623,12 @@
         <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -643,39 +649,13 @@
         <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="13" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change for one way booking
</commit_message>
<xml_diff>
--- a/src/test/java/resource/viadata.xlsx
+++ b/src/test/java/resource/viadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,36 @@
   </si>
   <si>
     <t>30/Mei/2024</t>
+  </si>
+  <si>
+    <t>Flight Found</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, TransNusa, Citilink, Scoot Airline, AirAsia Indonesia Airways, AirAsia Airways, Garuda, Singapore Airlines, Batik Air, Batik Air Malaysia, Lion Airways, Malaysia Airlines]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, TransNusa, AirAsia Indonesia Airways, Garuda, Nam Air, Pelita Air, Citilink, Super Air Jet, Lion Airways, Batik Air]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, Citilink, TransNusa, Jetstar Asia, Scoot Airline, AirAsia Indonesia Airways, AirAsia Airways, Batik Air, Batik Air Malaysia, Garuda, Singapore Airlines, Malaysia Airlines]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, Scoot Airline, Citilink, Jetstar Asia, TransNusa, AirAsia Indonesia Airways, AirAsia Airways, Singapore Airlines, Garuda, Batik Air, Batik Air Malaysia, Lion Airways, Malaysia Airlines]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, TransNusa, Jetstar Asia, Citilink, Scoot Airline, AirAsia Indonesia Airways, AirAsia Airways, Batik Air Malaysia, Batik Air, Lion Airways, Garuda, Singapore Airlines, Malaysia Airlines, Vietnam Airlines, Thai, China Airlines, Royal Brunei]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, TransNusa, AirAsia Indonesia Airways, Super Air Jet, Nam Air, Pelita Air, Citilink, Lion Airways, Batik Air, Garuda]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, TransNusa, Jetstar Asia, Citilink, Scoot Airline, AirAsia Airways, AirAsia Indonesia Airways, Batik Air, Batik Air Malaysia, Lion Airways, Garuda, Singapore Airlines, Royal Dutch, Malaysia Airlines, Philippine Airlines, Thai, China Airlines, Eva Airways, Royal Brunei]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, Scoot Airline, Jetstar Asia, Citilink, AirAsia Indonesia Airways, AirAsia Airways, TransNusa, Batik Air Malaysia, Batik Air, Lion Airways, Malaysia Airlines, Garuda, Singapore Airlines, Vietnam Airlines, Thai, China Airlines, Royal Brunei]</t>
+  </si>
+  <si>
+    <t>[Pilih Semua, Citilink, Scoot Airline, Jetstar Asia, AirAsia Airways, AirAsia Indonesia Airways, TransNusa, Royal Dutch, Batik Air Malaysia, Malaysia Airlines, Garuda, Singapore Airlines, Philippine Airlines, Thai, China Airlines, Eva Airways, Royal Brunei, Batik Air, Lion Airways]</t>
   </si>
 </sst>
 </file>
@@ -112,7 +142,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +172,21 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -240,22 +285,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,9 +601,10 @@
     <col min="6" max="6" customWidth="true" width="14.0"/>
     <col min="7" max="7" customWidth="true" width="14.42578125"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="6.06640625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="217.41796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -579,8 +629,11 @@
       <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -602,11 +655,14 @@
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="16" t="s">
         <v>22</v>
       </c>
+      <c r="I2" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -628,11 +684,14 @@
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="17" t="s">
         <v>22</v>
       </c>
+      <c r="I3" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -654,8 +713,11 @@
       <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="18" t="s">
         <v>23</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>